<commit_message>
Updated parametric study generator (excel book def)
</commit_message>
<xml_diff>
--- a/deap/mj_projects/definitionbooks/nsga1_zdt1_Xbinary_Mbinary SMALL.xlsx
+++ b/deap/mj_projects/definitionbooks/nsga1_zdt1_Xbinary_Mbinary SMALL.xlsx
@@ -4,17 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="3" r:id="rId1"/>
     <sheet name="Parameters" sheetId="11" r:id="rId2"/>
     <sheet name="Algorithm" sheetId="9" r:id="rId3"/>
-    <sheet name="Tabelle1" sheetId="12" r:id="rId4"/>
-    <sheet name="Operators" sheetId="7" r:id="rId5"/>
-    <sheet name="Range Variables" sheetId="1" r:id="rId6"/>
-    <sheet name="List Variables" sheetId="8" r:id="rId7"/>
-    <sheet name="Objectives" sheetId="4" r:id="rId8"/>
+    <sheet name="Operators" sheetId="7" r:id="rId4"/>
+    <sheet name="Range Variables" sheetId="1" r:id="rId5"/>
+    <sheet name="List Variables" sheetId="8" r:id="rId6"/>
+    <sheet name="Objectives" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -69,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="81">
   <si>
     <t>Yes</t>
   </si>
@@ -266,18 +265,9 @@
     <t>mj_operators</t>
   </si>
   <si>
-    <t>selTournamentDCD</t>
-  </si>
-  <si>
-    <t>Probability crossover</t>
-  </si>
-  <si>
     <t>mate</t>
   </si>
   <si>
-    <t>Probability mutation</t>
-  </si>
-  <si>
     <t>continue_run</t>
   </si>
   <si>
@@ -290,9 +280,6 @@
     <t>mj_mutPolynomialBounded</t>
   </si>
   <si>
-    <t>indpb</t>
-  </si>
-  <si>
     <t>evaluator</t>
   </si>
   <si>
@@ -309,6 +296,21 @@
   </si>
   <si>
     <t>UFTournSelection</t>
+  </si>
+  <si>
+    <t>Probability mutation individual</t>
+  </si>
+  <si>
+    <t>Probability crossover individual</t>
+  </si>
+  <si>
+    <t>Probability crossover allele</t>
+  </si>
+  <si>
+    <t>Probability mutation allele</t>
+  </si>
+  <si>
+    <t>in_memory</t>
   </si>
 </sst>
 </file>
@@ -687,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,10 +744,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -757,15 +767,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -795,7 +805,7 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>250</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>60</v>
@@ -803,7 +813,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B4">
         <v>0.9</v>
@@ -814,10 +824,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -825,10 +835,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -836,12 +846,23 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="8">
-        <v>3.3333333333333333E-2</v>
+        <v>79</v>
+      </c>
+      <c r="B7">
+        <v>0.03</v>
       </c>
       <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -861,18 +882,19 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,7 +910,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>58</v>
@@ -905,7 +927,7 @@
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -916,36 +938,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,18 +959,18 @@
         <v>57</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -985,7 +981,7 @@
         <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -993,12 +989,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,7 +1538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -1596,7 +1592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Post processing: - Generations are processed python after run completion, not in matlab - Post processing requires path to optimum front data
Excel pre-process:
- Refactored to use dict
- Added a section to remove redundant runs where crossover individual
prob was zero
</commit_message>
<xml_diff>
--- a/deap/mj_projects/definitionbooks/nsga1_zdt1_Xbinary_Mbinary SMALL.xlsx
+++ b/deap/mj_projects/definitionbooks/nsga1_zdt1_Xbinary_Mbinary SMALL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="3" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>Yes</t>
   </si>
@@ -124,6 +124,120 @@
     <t>var3</t>
   </si>
   <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>c:\TestProjectRoot</t>
+  </si>
+  <si>
+    <t>run_root_directory</t>
+  </si>
+  <si>
+    <t>run_name</t>
+  </si>
+  <si>
+    <t>version_folders</t>
+  </si>
+  <si>
+    <t>delete_folder</t>
+  </si>
+  <si>
+    <t>run_full_path</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>nsga2</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>mj_zdt1_decimal</t>
+  </si>
+  <si>
+    <t>tools</t>
+  </si>
+  <si>
+    <t>mj_evaluators</t>
+  </si>
+  <si>
+    <t>mj_algorithms</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>mutate</t>
+  </si>
+  <si>
+    <t>mj_operators</t>
+  </si>
+  <si>
+    <t>mate</t>
+  </si>
+  <si>
+    <t>continue_run</t>
+  </si>
+  <si>
+    <t>Crowding degree</t>
+  </si>
+  <si>
+    <t>mj_cxSimulatedBinaryBounded</t>
+  </si>
+  <si>
+    <t>mj_mutPolynomialBounded</t>
+  </si>
+  <si>
+    <t>evaluator</t>
+  </si>
+  <si>
+    <t>mj_utilities.util_general</t>
+  </si>
+  <si>
+    <t>evaluate_pop</t>
+  </si>
+  <si>
+    <t>life_cycle</t>
+  </si>
+  <si>
+    <t>selNSGA2revised</t>
+  </si>
+  <si>
+    <t>UFTournSelection</t>
+  </si>
+  <si>
+    <t>Probability mutation individual</t>
+  </si>
+  <si>
+    <t>Probability crossover individual</t>
+  </si>
+  <si>
+    <t>Probability crossover allele</t>
+  </si>
+  <si>
+    <t>Probability mutation allele</t>
+  </si>
+  <si>
+    <t>in_memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">path_opt_front </t>
+  </si>
+  <si>
+    <t>C:\Users\jon\git\deap1\examples\ga\pareto_front\zdt1_front.json</t>
+  </si>
+  <si>
     <t>var4</t>
   </si>
   <si>
@@ -146,171 +260,6 @@
   </si>
   <si>
     <t>var11</t>
-  </si>
-  <si>
-    <t>var12</t>
-  </si>
-  <si>
-    <t>var13</t>
-  </si>
-  <si>
-    <t>var14</t>
-  </si>
-  <si>
-    <t>var15</t>
-  </si>
-  <si>
-    <t>var16</t>
-  </si>
-  <si>
-    <t>var17</t>
-  </si>
-  <si>
-    <t>var18</t>
-  </si>
-  <si>
-    <t>var19</t>
-  </si>
-  <si>
-    <t>var20</t>
-  </si>
-  <si>
-    <t>var21</t>
-  </si>
-  <si>
-    <t>var22</t>
-  </si>
-  <si>
-    <t>var23</t>
-  </si>
-  <si>
-    <t>var24</t>
-  </si>
-  <si>
-    <t>var25</t>
-  </si>
-  <si>
-    <t>var26</t>
-  </si>
-  <si>
-    <t>var27</t>
-  </si>
-  <si>
-    <t>var28</t>
-  </si>
-  <si>
-    <t>var29</t>
-  </si>
-  <si>
-    <t>var30</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>c:\TestProjectRoot</t>
-  </si>
-  <si>
-    <t>run_root_directory</t>
-  </si>
-  <si>
-    <t>run_name</t>
-  </si>
-  <si>
-    <t>version_folders</t>
-  </si>
-  <si>
-    <t>delete_folder</t>
-  </si>
-  <si>
-    <t>run_full_path</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>nsga2</t>
-  </si>
-  <si>
-    <t>select</t>
-  </si>
-  <si>
-    <t>mj_zdt1_decimal</t>
-  </si>
-  <si>
-    <t>tools</t>
-  </si>
-  <si>
-    <t>mj_evaluators</t>
-  </si>
-  <si>
-    <t>mj_algorithms</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>mutate</t>
-  </si>
-  <si>
-    <t>mj_operators</t>
-  </si>
-  <si>
-    <t>mate</t>
-  </si>
-  <si>
-    <t>continue_run</t>
-  </si>
-  <si>
-    <t>Crowding degree</t>
-  </si>
-  <si>
-    <t>mj_cxSimulatedBinaryBounded</t>
-  </si>
-  <si>
-    <t>mj_mutPolynomialBounded</t>
-  </si>
-  <si>
-    <t>evaluator</t>
-  </si>
-  <si>
-    <t>mj_utilities.util_general</t>
-  </si>
-  <si>
-    <t>evaluate_pop</t>
-  </si>
-  <si>
-    <t>life_cycle</t>
-  </si>
-  <si>
-    <t>selNSGA2revised</t>
-  </si>
-  <si>
-    <t>UFTournSelection</t>
-  </si>
-  <si>
-    <t>Probability mutation individual</t>
-  </si>
-  <si>
-    <t>Probability crossover individual</t>
-  </si>
-  <si>
-    <t>Probability crossover allele</t>
-  </si>
-  <si>
-    <t>Probability mutation allele</t>
-  </si>
-  <si>
-    <t>in_memory</t>
   </si>
 </sst>
 </file>
@@ -689,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,23 +652,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B3" t="str">
         <f>CONCATENATE(B1,"\",B2)</f>
@@ -728,7 +677,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -736,7 +685,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -744,7 +693,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -752,10 +701,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -770,7 +727,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,13 +737,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -794,10 +751,10 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -805,15 +762,15 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>0.9</v>
@@ -824,7 +781,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="B5" s="8">
         <v>3.3333333333333333E-2</v>
@@ -835,7 +792,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -846,7 +803,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>0.03</v>
@@ -857,7 +814,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>20</v>
@@ -876,7 +833,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,46 +845,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -941,7 +898,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,35 +910,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -991,10 +948,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D31"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -1050,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -1067,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -1075,7 +1032,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -1084,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -1092,7 +1049,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -1101,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -1109,7 +1066,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -1118,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -1126,7 +1083,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -1135,7 +1092,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -1143,7 +1100,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -1152,7 +1109,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -1160,7 +1117,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -1169,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -1177,7 +1134,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -1186,7 +1143,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -1194,7 +1151,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -1203,332 +1160,9 @@
         <v>0</v>
       </c>
       <c r="D12" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E21" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E22" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E24" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E25" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="3">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="3">
-        <v>0</v>
-      </c>
-      <c r="D28" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E28" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="3">
-        <v>0</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E29" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="3">
-        <v>0</v>
-      </c>
-      <c r="D30" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E30" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="3">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E31" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1610,7 +1244,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>